<commit_message>
Ajustes y solicitud de video guion 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion08/Escaleta_LE_08_08_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion08/Escaleta_LE_08_08_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion08\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7050"/>
   </bookViews>
@@ -18,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
@@ -1266,6 +1271,132 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1328,132 +1459,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,7 +1565,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1595,7 +1600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1806,30 +1811,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L266" sqref="L266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="80" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="80" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="81" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="82" customWidth="1"/>
-    <col min="5" max="5" width="31" style="80" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="83" customWidth="1"/>
-    <col min="7" max="7" width="60" style="80" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="84" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="85" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="51" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" style="53" customWidth="1"/>
+    <col min="5" max="5" width="31" style="51" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" style="54" customWidth="1"/>
+    <col min="7" max="7" width="60" style="51" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="55" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="56" customWidth="1"/>
     <col min="10" max="10" width="37.5703125" style="3" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="80" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="80" customWidth="1"/>
-    <col min="15" max="15" width="37.85546875" style="85" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="86" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="85" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="51" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="51" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="57" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="56" customWidth="1"/>
     <col min="18" max="18" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.140625" style="3" customWidth="1"/>
     <col min="20" max="20" width="32.28515625" style="3" customWidth="1"/>
@@ -1838,100 +1843,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="26" t="s">
+      <c r="N1" s="80"/>
+      <c r="O1" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="60" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="33"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
       <c r="M2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="48"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="61"/>
     </row>
     <row r="3" spans="1:21" ht="46.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -1940,34 +1945,34 @@
       <c r="D3" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="28">
         <v>1</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="L3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="61"/>
-      <c r="N3" s="62" t="s">
+      <c r="M3" s="32"/>
+      <c r="N3" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="63" t="s">
+      <c r="O3" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="P3" s="64" t="s">
+      <c r="P3" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="22">
@@ -1987,10 +1992,10 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -2000,33 +2005,33 @@
         <v>123</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="65"/>
+      <c r="F4" s="36"/>
       <c r="G4" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="H4" s="66">
+      <c r="H4" s="37">
         <v>2</v>
       </c>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="60" t="s">
+      <c r="L4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62" t="s">
+      <c r="M4" s="33"/>
+      <c r="N4" s="33" t="s">
         <v>51</v>
       </c>
       <c r="O4" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="P4" s="64" t="s">
+      <c r="P4" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="22">
@@ -2046,10 +2051,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2059,33 +2064,33 @@
         <v>123</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="65"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="37">
         <v>3</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="60" t="s">
+      <c r="L5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62" t="s">
+      <c r="M5" s="33"/>
+      <c r="N5" s="33" t="s">
         <v>44</v>
       </c>
       <c r="O5" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="P5" s="64" t="s">
+      <c r="P5" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q5" s="22">
@@ -2105,10 +2110,10 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2118,33 +2123,33 @@
         <v>123</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="65"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="37">
         <v>4</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="33" t="s">
         <v>23</v>
       </c>
       <c r="O6" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="P6" s="64" t="s">
+      <c r="P6" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q6" s="22">
@@ -2164,10 +2169,10 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -2177,33 +2182,33 @@
         <v>123</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="65"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="37">
         <v>5</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="60" t="s">
+      <c r="L7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62" t="s">
+      <c r="M7" s="33"/>
+      <c r="N7" s="33" t="s">
         <v>28</v>
       </c>
       <c r="O7" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="P7" s="64" t="s">
+      <c r="P7" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="22">
@@ -2223,10 +2228,10 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -2236,33 +2241,33 @@
         <v>123</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="65"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="28">
         <v>6</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="60" t="s">
+      <c r="L8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62" t="s">
+      <c r="M8" s="33"/>
+      <c r="N8" s="33" t="s">
         <v>118</v>
       </c>
       <c r="O8" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="P8" s="64" t="s">
+      <c r="P8" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q8" s="22">
@@ -2282,10 +2287,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -2297,35 +2302,35 @@
       <c r="E9" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="37">
         <v>7</v>
       </c>
-      <c r="I9" s="68" t="s">
+      <c r="I9" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="K9" s="69" t="s">
+      <c r="K9" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62" t="s">
+      <c r="M9" s="33"/>
+      <c r="N9" s="33" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="P9" s="70" t="s">
+      <c r="P9" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q9" s="22">
@@ -2345,10 +2350,10 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -2360,35 +2365,35 @@
       <c r="E10" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="G10" s="67" t="s">
+      <c r="G10" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="37">
         <v>8</v>
       </c>
-      <c r="I10" s="68" t="s">
+      <c r="I10" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="K10" s="69" t="s">
+      <c r="K10" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62" t="s">
+      <c r="M10" s="33"/>
+      <c r="N10" s="33" t="s">
         <v>23</v>
       </c>
       <c r="O10" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="P10" s="70" t="s">
+      <c r="P10" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="22">
@@ -2408,10 +2413,10 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -2423,35 +2428,35 @@
       <c r="E11" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="G11" s="67" t="s">
+      <c r="G11" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="37">
         <v>9</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="K11" s="69" t="s">
+      <c r="K11" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="62" t="s">
+      <c r="M11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="62"/>
+      <c r="N11" s="33"/>
       <c r="O11" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="P11" s="70" t="s">
+      <c r="P11" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="22">
@@ -2471,10 +2476,10 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -2486,33 +2491,33 @@
       <c r="E12" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="65"/>
-      <c r="G12" s="67" t="s">
+      <c r="F12" s="36"/>
+      <c r="G12" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="H12" s="66">
+      <c r="H12" s="37">
         <v>10</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="I12" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="K12" s="69" t="s">
+      <c r="K12" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62" t="s">
+      <c r="M12" s="33"/>
+      <c r="N12" s="33" t="s">
         <v>31</v>
       </c>
       <c r="O12" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="P12" s="70" t="s">
+      <c r="P12" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="22">
@@ -2532,10 +2537,10 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -2547,33 +2552,33 @@
       <c r="E13" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="65"/>
-      <c r="G13" s="67" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H13" s="28">
         <v>11</v>
       </c>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="K13" s="69" t="s">
+      <c r="K13" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62" t="s">
+      <c r="M13" s="33"/>
+      <c r="N13" s="33" t="s">
         <v>27</v>
       </c>
       <c r="O13" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="P13" s="70" t="s">
+      <c r="P13" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q13" s="22">
@@ -2593,10 +2598,10 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -2608,33 +2613,33 @@
       <c r="E14" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="65"/>
-      <c r="G14" s="67" t="s">
+      <c r="F14" s="36"/>
+      <c r="G14" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="H14" s="66">
+      <c r="H14" s="37">
         <v>12</v>
       </c>
-      <c r="I14" s="68" t="s">
+      <c r="I14" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="K14" s="69" t="s">
+      <c r="K14" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="62" t="s">
+      <c r="M14" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="N14" s="62"/>
+      <c r="N14" s="33"/>
       <c r="O14" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="P14" s="70" t="s">
+      <c r="P14" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="22">
@@ -2654,10 +2659,10 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -2669,33 +2674,33 @@
       <c r="E15" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="65"/>
-      <c r="G15" s="67" t="s">
+      <c r="F15" s="36"/>
+      <c r="G15" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="H15" s="66">
+      <c r="H15" s="37">
         <v>13</v>
       </c>
-      <c r="I15" s="68" t="s">
+      <c r="I15" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="K15" s="69" t="s">
+      <c r="K15" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62" t="s">
+      <c r="M15" s="33"/>
+      <c r="N15" s="33" t="s">
         <v>121</v>
       </c>
       <c r="O15" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="P15" s="70" t="s">
+      <c r="P15" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q15" s="22">
@@ -2715,10 +2720,10 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -2730,33 +2735,33 @@
       <c r="E16" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="65"/>
-      <c r="G16" s="67" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="H16" s="66">
+      <c r="H16" s="37">
         <v>14</v>
       </c>
-      <c r="I16" s="68" t="s">
+      <c r="I16" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="K16" s="69" t="s">
+      <c r="K16" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="62"/>
-      <c r="N16" s="62" t="s">
+      <c r="M16" s="33"/>
+      <c r="N16" s="33" t="s">
         <v>34</v>
       </c>
       <c r="O16" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="P16" s="64" t="s">
+      <c r="P16" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q16" s="22">
@@ -2776,10 +2781,10 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -2791,33 +2796,33 @@
       <c r="E17" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="65"/>
-      <c r="G17" s="67" t="s">
+      <c r="F17" s="36"/>
+      <c r="G17" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="H17" s="66">
+      <c r="H17" s="37">
         <v>15</v>
       </c>
-      <c r="I17" s="68" t="s">
+      <c r="I17" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="K17" s="69" t="s">
+      <c r="K17" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L17" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62" t="s">
+      <c r="M17" s="33"/>
+      <c r="N17" s="33" t="s">
         <v>43</v>
       </c>
       <c r="O17" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="P17" s="64" t="s">
+      <c r="P17" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q17" s="22">
@@ -2837,10 +2842,10 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -2852,33 +2857,33 @@
       <c r="E18" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="65"/>
-      <c r="G18" s="67" t="s">
+      <c r="F18" s="36"/>
+      <c r="G18" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="H18" s="57">
+      <c r="H18" s="28">
         <v>16</v>
       </c>
-      <c r="I18" s="68" t="s">
+      <c r="I18" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="K18" s="69" t="s">
+      <c r="K18" s="40" t="s">
         <v>19</v>
       </c>
       <c r="L18" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M18" s="62" t="s">
+      <c r="M18" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="62"/>
+      <c r="N18" s="33"/>
       <c r="O18" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="P18" s="64" t="s">
+      <c r="P18" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q18" s="22">
@@ -2898,10 +2903,10 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -2913,31 +2918,31 @@
       <c r="E19" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="65"/>
-      <c r="G19" s="67" t="s">
+      <c r="F19" s="36"/>
+      <c r="G19" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="37">
         <v>17</v>
       </c>
-      <c r="I19" s="68" t="s">
+      <c r="I19" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="K19" s="69" t="s">
+      <c r="K19" s="40" t="s">
         <v>19</v>
       </c>
       <c r="L19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
       <c r="O19" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="P19" s="64" t="s">
+      <c r="P19" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q19" s="22">
@@ -2957,10 +2962,10 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -2972,31 +2977,31 @@
       <c r="E20" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="65"/>
-      <c r="G20" s="67" t="s">
+      <c r="F20" s="36"/>
+      <c r="G20" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="H20" s="66">
+      <c r="H20" s="37">
         <v>18</v>
       </c>
-      <c r="I20" s="68" t="s">
+      <c r="I20" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="K20" s="69" t="s">
+      <c r="K20" s="40" t="s">
         <v>19</v>
       </c>
       <c r="L20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
       <c r="O20" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="P20" s="64" t="s">
+      <c r="P20" s="35" t="s">
         <v>19</v>
       </c>
       <c r="Q20" s="22">
@@ -3016,10 +3021,10 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -3031,31 +3036,31 @@
       <c r="E21" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="65"/>
-      <c r="G21" s="67" t="s">
+      <c r="F21" s="36"/>
+      <c r="G21" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="H21" s="66">
+      <c r="H21" s="37">
         <v>19</v>
       </c>
-      <c r="I21" s="68" t="s">
+      <c r="I21" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="K21" s="69" t="s">
+      <c r="K21" s="40" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="62"/>
-      <c r="N21" s="62"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
       <c r="O21" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="P21" s="70" t="s">
+      <c r="P21" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q21" s="22">
@@ -3075,10 +3080,10 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -3090,33 +3095,33 @@
       <c r="E22" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="67" t="s">
+      <c r="F22" s="36"/>
+      <c r="G22" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="H22" s="66">
+      <c r="H22" s="37">
         <v>20</v>
       </c>
-      <c r="I22" s="68" t="s">
+      <c r="I22" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="K22" s="69" t="s">
+      <c r="K22" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="62" t="s">
+      <c r="M22" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="N22" s="62"/>
+      <c r="N22" s="33"/>
       <c r="O22" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="P22" s="70" t="s">
+      <c r="P22" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="22">
@@ -3136,10 +3141,10 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -3151,33 +3156,33 @@
       <c r="E23" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F23" s="65"/>
-      <c r="G23" s="67" t="s">
+      <c r="F23" s="36"/>
+      <c r="G23" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="H23" s="57">
+      <c r="H23" s="28">
         <v>21</v>
       </c>
-      <c r="I23" s="68" t="s">
+      <c r="I23" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="K23" s="69" t="s">
+      <c r="K23" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L23" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62" t="s">
+      <c r="M23" s="33"/>
+      <c r="N23" s="33" t="s">
         <v>24</v>
       </c>
       <c r="O23" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="P23" s="70" t="s">
+      <c r="P23" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="22">
@@ -3197,10 +3202,10 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -3212,33 +3217,33 @@
       <c r="E24" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="65"/>
-      <c r="G24" s="67" t="s">
+      <c r="F24" s="36"/>
+      <c r="G24" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="H24" s="66">
+      <c r="H24" s="37">
         <v>22</v>
       </c>
-      <c r="I24" s="68" t="s">
+      <c r="I24" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="K24" s="69" t="s">
+      <c r="K24" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L24" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62" t="s">
+      <c r="M24" s="33"/>
+      <c r="N24" s="33" t="s">
         <v>121</v>
       </c>
       <c r="O24" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="P24" s="70" t="s">
+      <c r="P24" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="22">
@@ -3258,10 +3263,10 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="150" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -3273,33 +3278,33 @@
       <c r="E25" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F25" s="65"/>
-      <c r="G25" s="67" t="s">
+      <c r="F25" s="36"/>
+      <c r="G25" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="H25" s="66">
+      <c r="H25" s="37">
         <v>23</v>
       </c>
-      <c r="I25" s="68" t="s">
+      <c r="I25" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="K25" s="69" t="s">
+      <c r="K25" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M25" s="62" t="s">
+      <c r="M25" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="N25" s="62"/>
+      <c r="N25" s="33"/>
       <c r="O25" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="P25" s="70" t="s">
+      <c r="P25" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q25" s="22">
@@ -3319,10 +3324,10 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -3334,33 +3339,33 @@
       <c r="E26" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F26" s="65"/>
-      <c r="G26" s="67" t="s">
+      <c r="F26" s="36"/>
+      <c r="G26" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="H26" s="57">
+      <c r="H26" s="28">
         <v>24</v>
       </c>
-      <c r="I26" s="68" t="s">
+      <c r="I26" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="K26" s="69" t="s">
+      <c r="K26" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L26" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62" t="s">
+      <c r="M26" s="33"/>
+      <c r="N26" s="33" t="s">
         <v>28</v>
       </c>
       <c r="O26" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="P26" s="70" t="s">
+      <c r="P26" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q26" s="22">
@@ -3380,10 +3385,10 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -3395,33 +3400,33 @@
       <c r="E27" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="67" t="s">
+      <c r="F27" s="36"/>
+      <c r="G27" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="H27" s="66">
+      <c r="H27" s="37">
         <v>25</v>
       </c>
-      <c r="I27" s="68" t="s">
+      <c r="I27" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J27" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="K27" s="69" t="s">
+      <c r="K27" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M27" s="62" t="s">
+      <c r="M27" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="N27" s="62"/>
+      <c r="N27" s="33"/>
       <c r="O27" s="20" t="s">
         <v>262</v>
       </c>
-      <c r="P27" s="70" t="s">
+      <c r="P27" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q27" s="22">
@@ -3441,10 +3446,10 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -3456,33 +3461,33 @@
       <c r="E28" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="65"/>
-      <c r="G28" s="67" t="s">
+      <c r="F28" s="36"/>
+      <c r="G28" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="H28" s="66">
+      <c r="H28" s="37">
         <v>26</v>
       </c>
-      <c r="I28" s="68" t="s">
+      <c r="I28" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J28" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="K28" s="69" t="s">
+      <c r="K28" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L28" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62" t="s">
+      <c r="M28" s="33"/>
+      <c r="N28" s="33" t="s">
         <v>33</v>
       </c>
       <c r="O28" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="P28" s="70" t="s">
+      <c r="P28" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q28" s="22">
@@ -3502,10 +3507,10 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -3517,33 +3522,33 @@
       <c r="E29" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F29" s="65"/>
-      <c r="G29" s="67" t="s">
+      <c r="F29" s="36"/>
+      <c r="G29" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="H29" s="57">
+      <c r="H29" s="28">
         <v>27</v>
       </c>
-      <c r="I29" s="68" t="s">
+      <c r="I29" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J29" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="K29" s="69" t="s">
+      <c r="K29" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="62"/>
-      <c r="N29" s="62" t="s">
+      <c r="M29" s="33"/>
+      <c r="N29" s="33" t="s">
         <v>30</v>
       </c>
       <c r="O29" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="P29" s="70" t="s">
+      <c r="P29" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q29" s="22">
@@ -3563,10 +3568,10 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -3578,33 +3583,33 @@
       <c r="E30" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F30" s="65"/>
-      <c r="G30" s="67" t="s">
+      <c r="F30" s="36"/>
+      <c r="G30" s="38" t="s">
         <v>271</v>
       </c>
-      <c r="H30" s="66">
+      <c r="H30" s="37">
         <v>28</v>
       </c>
-      <c r="I30" s="68" t="s">
+      <c r="I30" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J30" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="K30" s="69" t="s">
+      <c r="K30" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L30" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62" t="s">
+      <c r="M30" s="33"/>
+      <c r="N30" s="33" t="s">
         <v>121</v>
       </c>
       <c r="O30" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="P30" s="70" t="s">
+      <c r="P30" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="22">
@@ -3624,10 +3629,10 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -3637,33 +3642,33 @@
         <v>145</v>
       </c>
       <c r="E31" s="9"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="67" t="s">
+      <c r="F31" s="36"/>
+      <c r="G31" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="H31" s="66">
+      <c r="H31" s="37">
         <v>29</v>
       </c>
-      <c r="I31" s="68" t="s">
+      <c r="I31" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="K31" s="69" t="s">
+      <c r="K31" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M31" s="62" t="s">
+      <c r="M31" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="62"/>
+      <c r="N31" s="33"/>
       <c r="O31" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="P31" s="70" t="s">
+      <c r="P31" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="22">
@@ -3683,10 +3688,10 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -3698,33 +3703,33 @@
       <c r="E32" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F32" s="65"/>
-      <c r="G32" s="67" t="s">
+      <c r="F32" s="36"/>
+      <c r="G32" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="H32" s="57">
+      <c r="H32" s="28">
         <v>30</v>
       </c>
-      <c r="I32" s="68" t="s">
+      <c r="I32" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J32" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="K32" s="69" t="s">
+      <c r="K32" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L32" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="62"/>
-      <c r="N32" s="62" t="s">
+      <c r="M32" s="33"/>
+      <c r="N32" s="33" t="s">
         <v>43</v>
       </c>
       <c r="O32" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="P32" s="70" t="s">
+      <c r="P32" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="22">
@@ -3744,10 +3749,10 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -3759,33 +3764,33 @@
       <c r="E33" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F33" s="65"/>
-      <c r="G33" s="67" t="s">
+      <c r="F33" s="36"/>
+      <c r="G33" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="H33" s="66">
+      <c r="H33" s="37">
         <v>31</v>
       </c>
-      <c r="I33" s="68" t="s">
+      <c r="I33" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="K33" s="69" t="s">
+      <c r="K33" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L33" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M33" s="62"/>
-      <c r="N33" s="62" t="s">
+      <c r="M33" s="33"/>
+      <c r="N33" s="33" t="s">
         <v>22</v>
       </c>
       <c r="O33" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="P33" s="70" t="s">
+      <c r="P33" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="22">
@@ -3805,10 +3810,10 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -3820,54 +3825,54 @@
       <c r="E34" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="65"/>
-      <c r="G34" s="67" t="s">
+      <c r="F34" s="36"/>
+      <c r="G34" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="H34" s="66">
+      <c r="H34" s="37">
         <v>32</v>
       </c>
-      <c r="I34" s="68" t="s">
+      <c r="I34" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="K34" s="69" t="s">
+      <c r="K34" s="40" t="s">
         <v>19</v>
       </c>
       <c r="L34" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
       <c r="O34" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="P34" s="70" t="s">
+      <c r="P34" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="71">
+      <c r="Q34" s="42">
         <v>8</v>
       </c>
-      <c r="R34" s="72" t="s">
+      <c r="R34" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="S34" s="73" t="s">
+      <c r="S34" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="T34" s="74" t="s">
+      <c r="T34" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="U34" s="71" t="s">
+      <c r="U34" s="42" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -3879,33 +3884,33 @@
       <c r="E35" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="67" t="s">
+      <c r="F35" s="36"/>
+      <c r="G35" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="57">
+      <c r="H35" s="28">
         <v>33</v>
       </c>
-      <c r="I35" s="68" t="s">
+      <c r="I35" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J35" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="K35" s="69" t="s">
+      <c r="K35" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L35" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M35" s="62"/>
-      <c r="N35" s="62" t="s">
+      <c r="M35" s="33"/>
+      <c r="N35" s="33" t="s">
         <v>121</v>
       </c>
       <c r="O35" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="P35" s="70" t="s">
+      <c r="P35" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="22">
@@ -3925,10 +3930,10 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="53" t="s">
+      <c r="A36" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -3938,33 +3943,33 @@
         <v>148</v>
       </c>
       <c r="E36" s="9"/>
-      <c r="F36" s="65"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="H36" s="66">
+      <c r="H36" s="37">
         <v>34</v>
       </c>
-      <c r="I36" s="68" t="s">
+      <c r="I36" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="K36" s="69" t="s">
+      <c r="K36" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L36" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="75"/>
-      <c r="N36" s="62" t="s">
+      <c r="M36" s="46"/>
+      <c r="N36" s="33" t="s">
         <v>33</v>
       </c>
       <c r="O36" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="P36" s="70" t="s">
+      <c r="P36" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q36" s="22">
@@ -3984,10 +3989,10 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -3997,33 +4002,33 @@
         <v>148</v>
       </c>
       <c r="E37" s="9"/>
-      <c r="F37" s="65"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="H37" s="66">
+      <c r="H37" s="37">
         <v>35</v>
       </c>
-      <c r="I37" s="68" t="s">
+      <c r="I37" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J37" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="K37" s="69" t="s">
+      <c r="K37" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L37" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="75"/>
-      <c r="N37" s="62" t="s">
+      <c r="M37" s="46"/>
+      <c r="N37" s="33" t="s">
         <v>45</v>
       </c>
       <c r="O37" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="P37" s="70" t="s">
+      <c r="P37" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q37" s="22">
@@ -4043,10 +4048,10 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -4056,33 +4061,33 @@
         <v>148</v>
       </c>
       <c r="E38" s="9"/>
-      <c r="F38" s="65"/>
+      <c r="F38" s="36"/>
       <c r="G38" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="H38" s="57">
+      <c r="H38" s="28">
         <v>36</v>
       </c>
-      <c r="I38" s="68" t="s">
+      <c r="I38" s="39" t="s">
         <v>20</v>
       </c>
       <c r="J38" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="K38" s="69" t="s">
+      <c r="K38" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L38" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M38" s="75"/>
-      <c r="N38" s="62" t="s">
+      <c r="M38" s="46"/>
+      <c r="N38" s="33" t="s">
         <v>42</v>
       </c>
       <c r="O38" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="P38" s="70" t="s">
+      <c r="P38" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q38" s="22">
@@ -4102,10 +4107,10 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -4115,33 +4120,33 @@
         <v>148</v>
       </c>
       <c r="E39" s="9"/>
-      <c r="F39" s="65"/>
+      <c r="F39" s="36"/>
       <c r="G39" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="H39" s="66">
+      <c r="H39" s="37">
         <v>37</v>
       </c>
-      <c r="I39" s="68" t="s">
+      <c r="I39" s="39" t="s">
         <v>19</v>
       </c>
       <c r="J39" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="K39" s="69" t="s">
+      <c r="K39" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L39" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M39" s="62" t="s">
+      <c r="M39" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="N39" s="62"/>
+      <c r="N39" s="33"/>
       <c r="O39" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="P39" s="70" t="s">
+      <c r="P39" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q39" s="22">
@@ -4161,10 +4166,10 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -4174,42 +4179,42 @@
         <v>149</v>
       </c>
       <c r="E40" s="9"/>
-      <c r="F40" s="65"/>
+      <c r="F40" s="36"/>
       <c r="G40" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H40" s="66">
+      <c r="H40" s="37">
         <v>38</v>
       </c>
-      <c r="I40" s="68"/>
+      <c r="I40" s="39"/>
       <c r="J40" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="K40" s="69" t="s">
+      <c r="K40" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L40" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M40" s="76"/>
-      <c r="N40" s="76"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="47"/>
       <c r="O40" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="P40" s="70" t="s">
+      <c r="P40" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q40" s="77"/>
-      <c r="R40" s="78"/>
-      <c r="S40" s="77"/>
-      <c r="T40" s="79"/>
-      <c r="U40" s="77"/>
+      <c r="Q40" s="48"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="48"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="48"/>
     </row>
     <row r="41" spans="1:21" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -4219,31 +4224,31 @@
         <v>149</v>
       </c>
       <c r="E41" s="9"/>
-      <c r="F41" s="65"/>
+      <c r="F41" s="36"/>
       <c r="G41" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="H41" s="57">
+      <c r="H41" s="28">
         <v>39</v>
       </c>
-      <c r="I41" s="68"/>
+      <c r="I41" s="39"/>
       <c r="J41" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="K41" s="69" t="s">
+      <c r="K41" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L41" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="76"/>
-      <c r="N41" s="76" t="s">
+      <c r="M41" s="47"/>
+      <c r="N41" s="47" t="s">
         <v>32</v>
       </c>
       <c r="O41" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="P41" s="70" t="s">
+      <c r="P41" s="41" t="s">
         <v>19</v>
       </c>
       <c r="Q41" s="22">
@@ -4263,10 +4268,10 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="53" t="s">
+      <c r="A42" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="25" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -4276,32 +4281,32 @@
         <v>150</v>
       </c>
       <c r="E42" s="9"/>
-      <c r="F42" s="65"/>
+      <c r="F42" s="36"/>
       <c r="G42" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H42" s="66">
+      <c r="H42" s="37">
         <v>40</v>
       </c>
-      <c r="I42" s="68"/>
+      <c r="I42" s="39"/>
       <c r="J42" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="K42" s="69" t="s">
+      <c r="K42" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M42" s="76"/>
-      <c r="N42" s="76" t="s">
+      <c r="M42" s="47"/>
+      <c r="N42" s="47" t="s">
         <v>52</v>
       </c>
       <c r="O42" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="P42" s="70" t="s">
-        <v>19</v>
+      <c r="P42" s="41" t="s">
+        <v>20</v>
       </c>
       <c r="Q42" s="22">
         <v>6</v>
@@ -4333,187 +4338,187 @@
     <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="80" t="s">
+      <c r="A57" s="51" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="80" t="s">
+      <c r="A58" s="51" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="80" t="s">
+      <c r="A59" s="51" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="80" t="s">
+      <c r="A60" s="51" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="80" t="s">
+      <c r="A61" s="51" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="80" t="s">
+      <c r="A62" s="51" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="80" t="s">
+      <c r="A63" s="51" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="80" t="s">
+      <c r="A64" s="51" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="80" t="s">
+      <c r="A65" s="51" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="80" t="s">
+      <c r="A66" s="51" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="80" t="s">
+      <c r="A67" s="51" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="80" t="s">
+      <c r="A68" s="51" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="80" t="s">
+      <c r="A69" s="51" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="80" t="s">
+      <c r="A70" s="51" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="80" t="s">
+      <c r="A71" s="51" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="80" t="s">
+      <c r="A72" s="51" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="80" t="s">
+      <c r="A73" s="51" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="80" t="s">
+      <c r="A74" s="51" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="80" t="s">
+      <c r="A75" s="51" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="80" t="s">
+      <c r="A76" s="51" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="80" t="s">
+      <c r="A77" s="51" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="80" t="s">
+      <c r="A78" s="51" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="80" t="s">
+      <c r="A79" s="51" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="80" t="s">
+      <c r="A80" s="51" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="80" t="s">
+      <c r="A81" s="51" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="80" t="s">
+      <c r="A82" s="51" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="80" t="s">
+      <c r="A83" s="51" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="80" t="s">
+      <c r="A84" s="51" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="80" t="s">
+      <c r="A85" s="51" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="80" t="s">
+      <c r="A86" s="51" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="80" t="s">
+      <c r="A87" s="51" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="80" t="s">
+      <c r="A88" s="51" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="80" t="s">
+      <c r="A89" s="51" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="80" t="s">
+      <c r="A90" s="51" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="80" t="s">
+      <c r="A91" s="51" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="80" t="s">
+      <c r="A92" s="51" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="80" t="s">
+      <c r="A93" s="51" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4682,12 +4687,6 @@
     <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4702,6 +4701,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4736,7 +4741,7 @@
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I42 K3:K39 P3:P39</xm:sqref>
+          <xm:sqref>I3:I42 K3:K39 P3:P39 P42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4748,7 +4753,7 @@
           <x14:formula1>
             <xm:f>[3]DATOS!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>P40:P42 K40:N42</xm:sqref>
+          <xm:sqref>K40:N42 P40:P41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>